<commit_message>
new admin login for logs
</commit_message>
<xml_diff>
--- a/rfidexcelnew.xlsx
+++ b/rfidexcelnew.xlsx
@@ -3566,7 +3566,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4573,6 +4573,1634 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>E20241119701802024002172</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Paul Atreides</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>E20047030021642A023C3D52</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Vernier Caliper</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>BORROW</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>2025-11-07 08:44:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>E20241119701802024002172</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Paul Atreides</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>E2004702FFA1642A023C3D4A</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Micrometer</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>BORROW</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>2025-11-07 08:45:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>E20241119701802024002172</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Paul Atreides</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>E20047030021642A023C3D52</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Vernier Caliper</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>2025-11-07 08:45:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>E20241119701802024002172</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Paul Atreides</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>E2004702FFA1642A023C3D4A</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Micrometer</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Damaged</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>2025-11-07 08:45:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>E20047124741662E032E737C</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Kevin Flynn</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>E2004702FFA1642A023C3D4A</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Micrometer</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>BORROW</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>2025-11-07 08:47:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>E20047124741662E032E737C</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Kevin Flynn</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>E20047030021642A023C3D52</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Vernier Caliper</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>BORROW</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>2025-11-07 08:47:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>E20047124741662E032E737C</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Kevin Flynn</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>E2004702FFA1642A023C3D4A</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Micrometer</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>2025-11-07 08:48:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>E20047124741662E032E737C</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Kevin Flynn</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>E20047030021642A023C3D52</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Vernier Caliper</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>2025-11-07 08:48:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>E2004702FFA1642A023C3D4A</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Micrometer</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>BORROW</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>2025-11-07 08:54:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>E20047030021642A023C3D52</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Vernier Caliper</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>BORROW</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>2025-11-07 08:54:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>E20047030021642A023C3D52</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Vernier Caliper</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>2025-11-07 08:55:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>E2004702FFA1642A023C3D4A</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Micrometer</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>2025-11-07 08:55:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>E20047030021642A023C3D52</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Vernier Caliper</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>BORROW</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>2025-11-07 08:56:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>E2004702FFA1642A023C3D4A</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Micrometer</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>BORROW</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>2025-11-07 08:56:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>E2004702FFA1642A023C3D4A</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Micrometer</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>2025-11-07 08:56:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>E20047030021642A023C3D52</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Vernier Caliper</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>2025-11-07 08:56:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>E20047030021642A023C3D52</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Vernier Caliper</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>BORROW</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>2025-11-07 08:58:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>E2004702FFA1642A023C3D4A</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Micrometer</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>BORROW</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>2025-11-07 08:58:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>E20047030021642A023C3D52</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Vernier Caliper</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>2025-11-07 08:58:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>E2004702FFA1642A023C3D4A</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Micrometer</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Damaged</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>2025-11-07 08:58:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>E2004702FFA1642A023C3D4A</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Micrometer</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>BORROW</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>2025-11-07 09:00:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>E20047030021642A023C3D52</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Vernier Caliper</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>BORROW</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>2025-11-07 09:00:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>E20047030021642A023C3D52</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Vernier Caliper</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>2025-11-07 09:00:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>E2004702FFA1642A023C3D4A</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Micrometer</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>2025-11-07 09:01:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>E20047124741662E032E737C</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Kevin Flynn</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>E20047030021642A023C3D52</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Vernier Caliper</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>BORROW</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>2025-11-07 09:04:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>E20047124741662E032E737C</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Kevin Flynn</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>E2004702FFA1642A023C3D4A</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Micrometer</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>BORROW</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>2025-11-07 09:04:04</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>E20047124741662E032E737C</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Kevin Flynn</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>E2004702FFA1642A023C3D4A</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Micrometer</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>2025-11-07 09:04:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>E20047124741662E032E737C</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Kevin Flynn</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>E20047030021642A023C3D52</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Vernier Caliper</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>2025-11-07 09:04:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>E2004702FFA1642A023C3D4A</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Micrometer</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>BORROW</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>2025-11-07 09:08:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>E20047030021642A023C3D52</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Vernier Caliper</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>BORROW</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>2025-11-07 09:08:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>E2004702FFA1642A023C3D4A</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Micrometer</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>2025-11-07 09:09:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>E20047030021642A023C3D52</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Vernier Caliper</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>Damaged</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>2025-11-07 09:09:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>E20241119701802024002172</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Paul Atreides</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>E2004702FFA1642A023C3D4A</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Micrometer</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>BORROW</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>2025-11-07 09:09:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>E20241119701802024002172</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Paul Atreides</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>E20047030021642A023C3D52</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Vernier Caliper</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>BORROW</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>2025-11-07 09:09:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>E20241119701802024002172</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Paul Atreides</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>E20047030021642A023C3D52</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>Vernier Caliper</t>
+        </is>
+      </c>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>2025-11-07 09:10:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>E20241119701802024002172</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>Paul Atreides</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>E2004702FFA1642A023C3D4A</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>Micrometer</t>
+        </is>
+      </c>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>2025-11-07 09:12:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>E2004702FFA1642A023C3D4A</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>Micrometer</t>
+        </is>
+      </c>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>BORROW</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>2025-11-07 09:13:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>E20047030021642A023C3D52</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>Vernier Caliper</t>
+        </is>
+      </c>
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>BORROW</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>2025-11-07 09:13:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>E2004702FFA1642A023C3D4A</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>Micrometer</t>
+        </is>
+      </c>
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>2025-11-07 09:13:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>E20047030021642A023C3D52</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>Vernier Caliper</t>
+        </is>
+      </c>
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>2025-11-07 09:13:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>E20047030021642A023C3D52</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>Vernier Caliper</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>BORROW</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>2025-11-07 09:19:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>E2004702FFA1642A023C3D4A</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>Micrometer</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>BORROW</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>2025-11-07 09:19:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>E2004702FFA1642A023C3D4A</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>Micrometer</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>2025-11-07 09:19:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>E20241119701802024000520</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>Anakin Skywalker</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>E20047030021642A023C3D52</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>Vernier Caliper</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>RETURN</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>2025-11-07 09:19:34</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
new tool scan menu
added like a cart menu summary at the tool scan, to have more visibility on what they are scanning with the option to remove tool if accidental.
</commit_message>
<xml_diff>
--- a/rfidexcelnew.xlsx
+++ b/rfidexcelnew.xlsx
@@ -3566,7 +3566,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3644,7 +3644,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025-11-04 09:16:34</t>
+          <t>2025-11-07 10:03:40</t>
         </is>
       </c>
     </row>
@@ -3661,27 +3661,27 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>E20047030021642A023C3D52</t>
+          <t>E2004702FFA1642A023C3D4A</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Vernier Caliper</t>
+          <t>Micrometer</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>RETURN</t>
+          <t>BORROW</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025-11-04 09:16:55</t>
+          <t>2025-11-07 10:03:40</t>
         </is>
       </c>
     </row>
@@ -3698,27 +3698,27 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>E20047030021642A023C3D52</t>
+          <t>E2004702FFA1642A023C3D4A</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Vernier Caliper</t>
+          <t>Micrometer</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>BORROW</t>
+          <t>RETURN</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025-11-04 09:17:27</t>
+          <t>2025-11-07 10:03:57</t>
         </is>
       </c>
     </row>
@@ -3755,29 +3755,29 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025-11-04 09:18:03</t>
+          <t>2025-11-07 10:04:00</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>E20047124741662E032E737C</t>
+          <t>E20241119701802024002172</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Kevin Flynn</t>
+          <t>Paul Atreides</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>E20047030021642A023C3D52</t>
+          <t>E2004702FFA1642A023C3D4A</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Vernier Caliper</t>
+          <t>Micrometer</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -3792,19 +3792,19 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025-11-04 09:30:02</t>
+          <t>2025-11-07 10:04:56</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>E20047124741662E032E737C</t>
+          <t>E20241119701802024000520</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Kevin Flynn</t>
+          <t>Anakin Skywalker</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -3819,17 +3819,17 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>RETURN</t>
+          <t>BORROW</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025-11-04 09:54:20</t>
+          <t>2025-11-07 10:05:05</t>
         </is>
       </c>
     </row>
@@ -3846,39 +3846,39 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>E2004702FFA1642A023C3D4A</t>
+          <t>E20047030021642A023C3D52</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Micrometer</t>
+          <t>Vernier Caliper</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>BORROW</t>
+          <t>RETURN</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025-11-04 12:33:27</t>
+          <t>2025-11-07 10:05:17</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>E20241119701802024000520</t>
+          <t>E20241119701802024002172</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Anakin Skywalker</t>
+          <t>Paul Atreides</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -3903,29 +3903,29 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025-11-04 12:34:12</t>
+          <t>2025-11-07 10:05:24</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>E20047124741662E032E737C</t>
+          <t>E20241119701802024002172</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Kevin Flynn</t>
+          <t>Paul Atreides</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>E20047030021642A023C3D52</t>
+          <t>E2004702FFA1642A023C3D4A</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Vernier Caliper</t>
+          <t>Micrometer</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -3940,29 +3940,29 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025-11-04 12:40:52</t>
+          <t>2025-11-07 10:05:53</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>E20047124741662E032E737C</t>
+          <t>E20241119701802024002172</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Kevin Flynn</t>
+          <t>Paul Atreides</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>E20047030021642A023C3D52</t>
+          <t>E2004702FFA1642A023C3D4A</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Vernier Caliper</t>
+          <t>Micrometer</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -3977,29 +3977,29 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025-11-04 12:40:58</t>
+          <t>2025-11-07 10:05:59</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>E20047124741662E032E737C</t>
+          <t>E20241119701802024002172</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Kevin Flynn</t>
+          <t>Paul Atreides</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>E20047030021642A023C3D52</t>
+          <t>E2004702FFA1642A023C3D4A</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Vernier Caliper</t>
+          <t>Micrometer</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -4014,19 +4014,19 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025-11-04 12:43:04</t>
+          <t>2025-11-07 15:56:58</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>E20047124741662E032E737C</t>
+          <t>E20241119701802024002172</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Kevin Flynn</t>
+          <t>Paul Atreides</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -4041,29 +4041,29 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>RETURN</t>
+          <t>BORROW</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Damaged</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025-11-04 12:43:09</t>
+          <t>2025-11-07 15:57:09</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>E20047124741662E032E737C</t>
+          <t>E20241119701802024002172</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Kevin Flynn</t>
+          <t>Paul Atreides</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -4078,29 +4078,29 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>BORROW</t>
+          <t>RETURN</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025-11-04 12:53:21</t>
+          <t>2025-11-07 15:57:22</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>E20047124741662E032E737C</t>
+          <t>E20241119701802024002172</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Kevin Flynn</t>
+          <t>Paul Atreides</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -4115,29 +4115,29 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>BORROW</t>
+          <t>RETURN</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Damaged</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025-11-04 13:04:46</t>
+          <t>2025-11-07 15:57:28</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>E20047124741662E032E737C</t>
+          <t>E20241119701802024002172</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Kevin Flynn</t>
+          <t>Paul Atreides</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -4152,39 +4152,39 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>RETURN</t>
+          <t>BORROW</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Damaged</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025-11-04 13:05:06</t>
+          <t>2025-11-07 16:00:12</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>E20047124741662E032E737C</t>
+          <t>E20241119701802024002172</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Kevin Flynn</t>
+          <t>Paul Atreides</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>E20047030021642A023C3D52</t>
+          <t>E2004702FFA1642A023C3D4A</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Vernier Caliper</t>
+          <t>Micrometer</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -4199,29 +4199,29 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025-11-04 13:09:46</t>
+          <t>2025-11-07 16:45:28</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>E20047124741662E032E737C</t>
+          <t>E20241119701802024002172</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Kevin Flynn</t>
+          <t>Paul Atreides</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>E20047030021642A023C3D52</t>
+          <t>E2004702FFA1642A023C3D4A</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Vernier Caliper</t>
+          <t>Micrometer</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -4236,29 +4236,29 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025-11-04 13:53:50</t>
+          <t>2025-11-07 16:46:20</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>E20047124741662E032E737C</t>
+          <t>E20241119701802024002172</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Kevin Flynn</t>
+          <t>Paul Atreides</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>E20047030021642A023C3D52</t>
+          <t>E2004702FFA1642A023C3D4A</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Vernier Caliper</t>
+          <t>Micrometer</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -4273,7 +4273,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025-11-05 08:33:40</t>
+          <t>2025-11-11 13:08:29</t>
         </is>
       </c>
     </row>
@@ -4310,7 +4310,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025-11-05 08:35:01</t>
+          <t>2025-11-11 13:09:06</t>
         </is>
       </c>
     </row>
@@ -4327,76 +4327,76 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>E2004702FFA1642A023C3D4A</t>
+          <t>E20047030021642A023C3D52</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Micrometer</t>
+          <t>Vernier Caliper</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>RETURN</t>
+          <t>BORROW</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Damaged</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025-11-05 09:10:32</t>
+          <t>2025-11-11 13:09:06</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>E20047124741662E032E737C</t>
+          <t>E20241119701802024000520</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Kevin Flynn</t>
+          <t>Anakin Skywalker</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>E2004702FFA1642A023C3D4A</t>
+          <t>E20047030021642A023C3D52</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Micrometer</t>
+          <t>Vernier Caliper</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>BORROW</t>
+          <t>RETURN</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025-11-05 09:15:30</t>
+          <t>2025-11-11 13:12:12</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>E20047124741662E032E737C</t>
+          <t>E20241119701802024000520</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Kevin Flynn</t>
+          <t>Anakin Skywalker</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -4421,29 +4421,29 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025-11-05 09:15:48</t>
+          <t>2025-11-11 13:12:17</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>E20047124741662E032E737C</t>
+          <t>E20241119701802024002172</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Kevin Flynn</t>
+          <t>Paul Atreides</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>E2004702FFA1642A023C3D4A</t>
+          <t>E20047030021642A023C3D52</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Micrometer</t>
+          <t>Vernier Caliper</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -4458,19 +4458,19 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2025-11-05 09:16:19</t>
+          <t>2025-11-11 13:20:30</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>E20047124741662E032E737C</t>
+          <t>E20241119701802024002172</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Kevin Flynn</t>
+          <t>Paul Atreides</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -4485,66 +4485,66 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>RETURN</t>
+          <t>BORROW</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Damaged</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025-11-05 09:16:40</t>
+          <t>2025-11-11 13:20:30</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>E20047124741662E032E737C</t>
+          <t>E20241119701802024002172</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Kevin Flynn</t>
+          <t>Paul Atreides</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>E20047030021642A023C3D52</t>
+          <t>E2004702FFA1642A023C3D4A</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Vernier Caliper</t>
+          <t>Micrometer</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>BORROW</t>
+          <t>RETURN</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025-11-05 12:33:13</t>
+          <t>2025-11-11 13:32:01</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>E20047124741662E032E737C</t>
+          <t>E20241119701802024002172</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Kevin Flynn</t>
+          <t>Paul Atreides</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -4564,12 +4564,12 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Damaged</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025-11-05 12:33:24</t>
+          <t>2025-11-11 13:32:09</t>
         </is>
       </c>
     </row>
@@ -4606,7 +4606,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2025-11-07 08:44:57</t>
+          <t>2025-11-11 13:33:36</t>
         </is>
       </c>
     </row>
@@ -4623,1581 +4623,64 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>E2004702FFA1642A023C3D4A</t>
+          <t>E20047030021642A023C3D52</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Micrometer</t>
+          <t>Vernier Caliper</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>BORROW</t>
+          <t>RETURN</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>Good</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2025-11-07 08:45:05</t>
+          <t>2025-11-11 13:33:51</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>E20241119701802024002172</t>
+          <t>E20241119701802024000520</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Paul Atreides</t>
+          <t>Anakin Skywalker</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>E20047030021642A023C3D52</t>
+          <t>E2004702FFA1642A023C3D4A</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Vernier Caliper</t>
+          <t>Micrometer</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>RETURN</t>
+          <t>BORROW</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Good</t>
+          <t>-</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2025-11-07 08:45:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>E20241119701802024002172</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Paul Atreides</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>E2004702FFA1642A023C3D4A</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Micrometer</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>Damaged</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>2025-11-07 08:45:33</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>E20047124741662E032E737C</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Kevin Flynn</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>E2004702FFA1642A023C3D4A</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>Micrometer</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>BORROW</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>2025-11-07 08:47:33</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>E20047124741662E032E737C</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Kevin Flynn</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>E20047030021642A023C3D52</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Vernier Caliper</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>BORROW</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>2025-11-07 08:47:34</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>E20047124741662E032E737C</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Kevin Flynn</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>E2004702FFA1642A023C3D4A</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>Micrometer</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>2025-11-07 08:48:05</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>E20047124741662E032E737C</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Kevin Flynn</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>E20047030021642A023C3D52</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Vernier Caliper</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>2025-11-07 08:48:09</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>E2004702FFA1642A023C3D4A</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>Micrometer</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>BORROW</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>2025-11-07 08:54:32</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>E20047030021642A023C3D52</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Vernier Caliper</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>BORROW</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>2025-11-07 08:54:45</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>E20047030021642A023C3D52</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>Vernier Caliper</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>2025-11-07 08:55:21</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>E2004702FFA1642A023C3D4A</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>Micrometer</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>2025-11-07 08:55:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>E20047030021642A023C3D52</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>Vernier Caliper</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>BORROW</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>2025-11-07 08:56:34</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>E2004702FFA1642A023C3D4A</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>Micrometer</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>BORROW</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>2025-11-07 08:56:36</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>E2004702FFA1642A023C3D4A</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>Micrometer</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>2025-11-07 08:56:46</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>E20047030021642A023C3D52</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>Vernier Caliper</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>2025-11-07 08:56:55</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>E20047030021642A023C3D52</t>
-        </is>
-      </c>
-      <c r="D44" t="inlineStr">
-        <is>
-          <t>Vernier Caliper</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>BORROW</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>2025-11-07 08:58:22</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>E2004702FFA1642A023C3D4A</t>
-        </is>
-      </c>
-      <c r="D45" t="inlineStr">
-        <is>
-          <t>Micrometer</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>BORROW</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>2025-11-07 08:58:23</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>E20047030021642A023C3D52</t>
-        </is>
-      </c>
-      <c r="D46" t="inlineStr">
-        <is>
-          <t>Vernier Caliper</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>2025-11-07 08:58:32</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>E2004702FFA1642A023C3D4A</t>
-        </is>
-      </c>
-      <c r="D47" t="inlineStr">
-        <is>
-          <t>Micrometer</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>Damaged</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>2025-11-07 08:58:40</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>E2004702FFA1642A023C3D4A</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Micrometer</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>BORROW</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>2025-11-07 09:00:45</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>E20047030021642A023C3D52</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>Vernier Caliper</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>BORROW</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>2025-11-07 09:00:48</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>E20047030021642A023C3D52</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Vernier Caliper</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>2025-11-07 09:00:54</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>E2004702FFA1642A023C3D4A</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>Micrometer</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>2025-11-07 09:01:19</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>E20047124741662E032E737C</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>Kevin Flynn</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>E20047030021642A023C3D52</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>Vernier Caliper</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>BORROW</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>2025-11-07 09:04:04</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>E20047124741662E032E737C</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>Kevin Flynn</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>E2004702FFA1642A023C3D4A</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>Micrometer</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>BORROW</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>2025-11-07 09:04:04</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>E20047124741662E032E737C</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Kevin Flynn</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>E2004702FFA1642A023C3D4A</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>Micrometer</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>2025-11-07 09:04:14</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>E20047124741662E032E737C</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Kevin Flynn</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>E20047030021642A023C3D52</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>Vernier Caliper</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>2025-11-07 09:04:20</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>E2004702FFA1642A023C3D4A</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>Micrometer</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>BORROW</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>2025-11-07 09:08:43</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>E20047030021642A023C3D52</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>Vernier Caliper</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>BORROW</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>2025-11-07 09:08:45</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>E2004702FFA1642A023C3D4A</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>Micrometer</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>2025-11-07 09:09:38</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>E20047030021642A023C3D52</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>Vernier Caliper</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>Damaged</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>2025-11-07 09:09:43</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>E20241119701802024002172</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>Paul Atreides</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>E2004702FFA1642A023C3D4A</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>Micrometer</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>BORROW</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>2025-11-07 09:09:51</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>E20241119701802024002172</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>Paul Atreides</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>E20047030021642A023C3D52</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>Vernier Caliper</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>BORROW</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>2025-11-07 09:09:53</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>E20241119701802024002172</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>Paul Atreides</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>E20047030021642A023C3D52</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>Vernier Caliper</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>2025-11-07 09:10:28</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>E20241119701802024002172</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>Paul Atreides</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>E2004702FFA1642A023C3D4A</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>Micrometer</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>2025-11-07 09:12:58</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>E2004702FFA1642A023C3D4A</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>Micrometer</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>BORROW</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>2025-11-07 09:13:11</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>E20047030021642A023C3D52</t>
-        </is>
-      </c>
-      <c r="D65" t="inlineStr">
-        <is>
-          <t>Vernier Caliper</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>BORROW</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>2025-11-07 09:13:13</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>E2004702FFA1642A023C3D4A</t>
-        </is>
-      </c>
-      <c r="D66" t="inlineStr">
-        <is>
-          <t>Micrometer</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>2025-11-07 09:13:28</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>E20047030021642A023C3D52</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>Vernier Caliper</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>2025-11-07 09:13:42</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>E20047030021642A023C3D52</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>Vernier Caliper</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>BORROW</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>2025-11-07 09:19:19</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>E2004702FFA1642A023C3D4A</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>Micrometer</t>
-        </is>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>BORROW</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>2025-11-07 09:19:20</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>E2004702FFA1642A023C3D4A</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>Micrometer</t>
-        </is>
-      </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>2025-11-07 09:19:31</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>E20241119701802024000520</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>Anakin Skywalker</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>E20047030021642A023C3D52</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>Vernier Caliper</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>RETURN</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>Good</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>2025-11-07 09:19:34</t>
+          <t>2025-11-11 13:39:01</t>
         </is>
       </c>
     </row>

</xml_diff>